<commit_message>
full of errors extra attempts
</commit_message>
<xml_diff>
--- a/bbtest.xlsx
+++ b/bbtest.xlsx
@@ -2498,25 +2498,25 @@
         <v>4</v>
       </c>
       <c r="C2">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
         <v>8</v>
       </c>
-      <c r="E2">
-        <v>2</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
       <c r="G2">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J2">
         <v>0</v>
@@ -2570,7 +2570,7 @@
         <v>0</v>
       </c>
       <c r="AA2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB2">
         <v>0</v>
@@ -2612,7 +2612,7 @@
         <v>0</v>
       </c>
       <c r="AO2">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:41">
@@ -2620,7 +2620,7 @@
         <v>106</v>
       </c>
       <c r="B3">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="C3">
         <v>6</v>
@@ -3760,13 +3760,13 @@
         <v>0</v>
       </c>
       <c r="G12">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H12">
         <v>0</v>
       </c>
       <c r="I12">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J12">
         <v>0</v>
@@ -4266,7 +4266,7 @@
         <v>2</v>
       </c>
       <c r="I16">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J16">
         <v>0</v>
@@ -4510,13 +4510,13 @@
         <v>0</v>
       </c>
       <c r="G18">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H18">
         <v>0</v>
       </c>
       <c r="I18">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J18">
         <v>0</v>
@@ -4737,7 +4737,7 @@
         <v>0</v>
       </c>
       <c r="AO19">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:41">
@@ -5862,7 +5862,7 @@
         <v>0</v>
       </c>
       <c r="AO28">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:41">
@@ -6016,7 +6016,7 @@
         <v>0</v>
       </c>
       <c r="I30">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J30">
         <v>0</v>
@@ -6112,7 +6112,7 @@
         <v>0</v>
       </c>
       <c r="AO30">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="31" spans="1:41">
@@ -7487,7 +7487,7 @@
         <v>0</v>
       </c>
       <c r="AO41">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="42" spans="1:41">
@@ -8754,7 +8754,7 @@
         <v>0</v>
       </c>
       <c r="E52">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F52">
         <v>0</v>
@@ -8778,7 +8778,7 @@
         <v>0</v>
       </c>
       <c r="M52">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="N52">
         <v>0</v>
@@ -10011,7 +10011,7 @@
         <v>105</v>
       </c>
       <c r="B2">
-        <v>4910</v>
+        <v>8680</v>
       </c>
       <c r="C2">
         <v>80</v>
@@ -10019,11 +10019,17 @@
       <c r="D2">
         <v>180</v>
       </c>
-      <c r="E2">
-        <v>280</v>
-      </c>
-      <c r="F2">
-        <v>390</v>
+      <c r="G2">
+        <v>480</v>
+      </c>
+      <c r="H2">
+        <v>580</v>
+      </c>
+      <c r="J2">
+        <v>780</v>
+      </c>
+      <c r="AB2">
+        <v>2600</v>
       </c>
       <c r="AP2">
         <v>3980</v>
@@ -10115,7 +10121,7 @@
         <v>109</v>
       </c>
       <c r="B6">
-        <v>2570</v>
+        <v>6550</v>
       </c>
       <c r="C6">
         <v>100</v>
@@ -10131,6 +10137,9 @@
       </c>
       <c r="O6">
         <v>1290</v>
+      </c>
+      <c r="AP6">
+        <v>3980</v>
       </c>
     </row>
     <row r="7" spans="1:42">
@@ -10138,7 +10147,7 @@
         <v>110</v>
       </c>
       <c r="B7">
-        <v>3140</v>
+        <v>7120</v>
       </c>
       <c r="G7">
         <v>480</v>
@@ -10151,6 +10160,9 @@
       </c>
       <c r="N7">
         <v>1190</v>
+      </c>
+      <c r="AP7">
+        <v>3980</v>
       </c>
     </row>
     <row r="8" spans="1:42">
@@ -10181,7 +10193,7 @@
         <v>112</v>
       </c>
       <c r="B9">
-        <v>7030</v>
+        <v>11010</v>
       </c>
       <c r="K9">
         <v>880</v>
@@ -10197,6 +10209,9 @@
       </c>
       <c r="U9">
         <v>1900</v>
+      </c>
+      <c r="AP9">
+        <v>3980</v>
       </c>
     </row>
     <row r="10" spans="1:42">
@@ -10247,7 +10262,13 @@
         <v>115</v>
       </c>
       <c r="B12">
-        <v>14790</v>
+        <v>16150</v>
+      </c>
+      <c r="H12">
+        <v>580</v>
+      </c>
+      <c r="J12">
+        <v>780</v>
       </c>
       <c r="AJ12">
         <v>3400</v>
@@ -10363,11 +10384,14 @@
         <v>119</v>
       </c>
       <c r="B16">
-        <v>4150</v>
+        <v>4930</v>
       </c>
       <c r="I16">
         <v>690</v>
       </c>
+      <c r="J16">
+        <v>780</v>
+      </c>
       <c r="L16">
         <v>980</v>
       </c>
@@ -10378,7 +10402,7 @@
         <v>1290</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:42">
       <c r="A17" t="s">
         <v>120</v>
       </c>
@@ -10389,26 +10413,35 @@
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:42">
       <c r="A18" t="s">
         <v>121</v>
       </c>
       <c r="B18">
-        <v>80</v>
+        <v>1440</v>
       </c>
       <c r="C18">
         <v>80</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="H18">
+        <v>580</v>
+      </c>
+      <c r="J18">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="19" spans="1:42">
       <c r="A19" t="s">
         <v>122</v>
       </c>
       <c r="B19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
+        <v>3980</v>
+      </c>
+      <c r="AP19">
+        <v>3980</v>
+      </c>
+    </row>
+    <row r="20" spans="1:42">
       <c r="A20" t="s">
         <v>123</v>
       </c>
@@ -10416,7 +10449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:42">
       <c r="A21" t="s">
         <v>124</v>
       </c>
@@ -10424,7 +10457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:42">
       <c r="A22" t="s">
         <v>125</v>
       </c>
@@ -10432,7 +10465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:42">
       <c r="A23" t="s">
         <v>126</v>
       </c>
@@ -10440,7 +10473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:42">
       <c r="A24" t="s">
         <v>127</v>
       </c>
@@ -10448,7 +10481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:42">
       <c r="A25" t="s">
         <v>128</v>
       </c>
@@ -10456,7 +10489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:42">
       <c r="A26" t="s">
         <v>129</v>
       </c>
@@ -10464,7 +10497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:42">
       <c r="A27" t="s">
         <v>130</v>
       </c>
@@ -10472,15 +10505,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:42">
       <c r="A28" t="s">
         <v>131</v>
       </c>
       <c r="B28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
+        <v>3980</v>
+      </c>
+      <c r="AP28">
+        <v>3980</v>
+      </c>
+    </row>
+    <row r="29" spans="1:42">
       <c r="A29" t="s">
         <v>132</v>
       </c>
@@ -10488,15 +10524,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:42">
       <c r="A30" t="s">
         <v>133</v>
       </c>
       <c r="B30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
+        <v>4760</v>
+      </c>
+      <c r="J30">
+        <v>780</v>
+      </c>
+      <c r="AP30">
+        <v>3980</v>
+      </c>
+    </row>
+    <row r="31" spans="1:42">
       <c r="A31" t="s">
         <v>134</v>
       </c>
@@ -10504,7 +10546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:42">
       <c r="A32" t="s">
         <v>135</v>
       </c>
@@ -10643,7 +10685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:14">
       <c r="A49" t="s">
         <v>152</v>
       </c>
@@ -10651,7 +10693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:14">
       <c r="A50" t="s">
         <v>153</v>
       </c>
@@ -10659,7 +10701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" spans="1:14">
       <c r="A51" t="s">
         <v>154</v>
       </c>
@@ -10667,15 +10709,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
+    <row r="52" spans="1:14">
       <c r="A52" t="s">
         <v>155</v>
       </c>
       <c r="B52">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2">
+        <v>1560</v>
+      </c>
+      <c r="F52">
+        <v>380</v>
+      </c>
+      <c r="N52">
+        <v>1180</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14">
       <c r="A53" t="s">
         <v>156</v>
       </c>
@@ -10683,7 +10731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
+    <row r="54" spans="1:14">
       <c r="A54" t="s">
         <v>157</v>
       </c>
@@ -10691,7 +10739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
+    <row r="55" spans="1:14">
       <c r="A55" t="s">
         <v>158</v>
       </c>
@@ -10699,7 +10747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
+    <row r="56" spans="1:14">
       <c r="A56" t="s">
         <v>159</v>
       </c>
@@ -10707,7 +10755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
+    <row r="57" spans="1:14">
       <c r="A57" t="s">
         <v>160</v>
       </c>
@@ -10715,7 +10763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
+    <row r="58" spans="1:14">
       <c r="A58" t="s">
         <v>161</v>
       </c>
@@ -10723,7 +10771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
+    <row r="59" spans="1:14">
       <c r="A59" t="s">
         <v>162</v>
       </c>
@@ -10731,7 +10779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
+    <row r="60" spans="1:14">
       <c r="A60" t="s">
         <v>163</v>
       </c>

</xml_diff>

<commit_message>
Bug Fixes and Semantics Changes
</commit_message>
<xml_diff>
--- a/bbtest.xlsx
+++ b/bbtest.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="1" r:id="rId1"/>
-    <sheet name="Attempts" sheetId="2" r:id="rId2"/>
+    <sheet name="Send Attempt" sheetId="2" r:id="rId2"/>
     <sheet name="Scores" sheetId="3" r:id="rId3"/>
     <sheet name="LeaderBoard" sheetId="4" r:id="rId4"/>
   </sheets>
@@ -2501,22 +2501,22 @@
         <v>6</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G2">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
       <c r="I2">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="J2">
         <v>0</v>
@@ -2570,7 +2570,7 @@
         <v>0</v>
       </c>
       <c r="AA2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB2">
         <v>0</v>
@@ -2612,7 +2612,7 @@
         <v>0</v>
       </c>
       <c r="AO2">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:41">
@@ -2620,28 +2620,28 @@
         <v>106</v>
       </c>
       <c r="B3">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
       <c r="I3">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="J3">
         <v>0</v>
@@ -2737,7 +2737,7 @@
         <v>0</v>
       </c>
       <c r="AO3">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:41">
@@ -2745,13 +2745,13 @@
         <v>107</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -2763,7 +2763,7 @@
         <v>0</v>
       </c>
       <c r="H4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I4">
         <v>0</v>
@@ -2775,10 +2775,10 @@
         <v>0</v>
       </c>
       <c r="L4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N4">
         <v>0</v>
@@ -2862,7 +2862,7 @@
         <v>0</v>
       </c>
       <c r="AO4">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:41">
@@ -2873,13 +2873,13 @@
         <v>0</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -2995,13 +2995,13 @@
         <v>109</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -3013,7 +3013,7 @@
         <v>0</v>
       </c>
       <c r="H6">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I6">
         <v>0</v>
@@ -3031,7 +3031,7 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O6">
         <v>0</v>
@@ -3112,7 +3112,7 @@
         <v>0</v>
       </c>
       <c r="AO6">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:41">
@@ -3132,16 +3132,16 @@
         <v>0</v>
       </c>
       <c r="F7">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G7">
         <v>0</v>
       </c>
       <c r="H7">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J7">
         <v>0</v>
@@ -3153,7 +3153,7 @@
         <v>0</v>
       </c>
       <c r="M7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N7">
         <v>0</v>
@@ -3237,7 +3237,7 @@
         <v>0</v>
       </c>
       <c r="AO7">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:41">
@@ -3257,7 +3257,7 @@
         <v>0</v>
       </c>
       <c r="F8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -3272,16 +3272,16 @@
         <v>0</v>
       </c>
       <c r="K8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L8">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O8">
         <v>0</v>
@@ -3394,13 +3394,13 @@
         <v>0</v>
       </c>
       <c r="J9">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K9">
         <v>0</v>
       </c>
       <c r="L9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M9">
         <v>0</v>
@@ -3409,7 +3409,7 @@
         <v>0</v>
       </c>
       <c r="O9">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="P9">
         <v>0</v>
@@ -3421,10 +3421,10 @@
         <v>0</v>
       </c>
       <c r="S9">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="T9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U9">
         <v>0</v>
@@ -3487,7 +3487,7 @@
         <v>0</v>
       </c>
       <c r="AO9">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:41">
@@ -3495,7 +3495,7 @@
         <v>113</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -3513,19 +3513,19 @@
         <v>0</v>
       </c>
       <c r="H10">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I10">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J10">
         <v>0</v>
       </c>
       <c r="K10">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L10">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M10">
         <v>0</v>
@@ -3686,25 +3686,25 @@
         <v>0</v>
       </c>
       <c r="X11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Y11">
         <v>0</v>
       </c>
       <c r="Z11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AA11">
         <v>0</v>
       </c>
       <c r="AB11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AC11">
         <v>0</v>
       </c>
       <c r="AD11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AE11">
         <v>0</v>
@@ -3760,13 +3760,13 @@
         <v>0</v>
       </c>
       <c r="G12">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H12">
         <v>0</v>
       </c>
       <c r="I12">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="J12">
         <v>0</v>
@@ -3844,25 +3844,25 @@
         <v>0</v>
       </c>
       <c r="AI12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ12">
         <v>0</v>
       </c>
       <c r="AK12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL12">
         <v>0</v>
       </c>
       <c r="AM12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN12">
         <v>0</v>
       </c>
       <c r="AO12">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:41">
@@ -3915,7 +3915,7 @@
         <v>0</v>
       </c>
       <c r="Q13">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="R13">
         <v>0</v>
@@ -3969,16 +3969,16 @@
         <v>0</v>
       </c>
       <c r="AI13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ13">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AK13">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AL13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM13">
         <v>0</v>
@@ -4046,7 +4046,7 @@
         <v>0</v>
       </c>
       <c r="S14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T14">
         <v>0</v>
@@ -4073,25 +4073,25 @@
         <v>0</v>
       </c>
       <c r="AB14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AC14">
         <v>0</v>
       </c>
       <c r="AD14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AE14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AG14">
         <v>0</v>
       </c>
       <c r="AH14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AI14">
         <v>0</v>
@@ -4106,13 +4106,13 @@
         <v>0</v>
       </c>
       <c r="AM14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AN14">
         <v>0</v>
       </c>
       <c r="AO14">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:41">
@@ -4120,13 +4120,13 @@
         <v>118</v>
       </c>
       <c r="B15">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C15">
         <v>0</v>
       </c>
       <c r="D15">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -4138,13 +4138,13 @@
         <v>0</v>
       </c>
       <c r="H15">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I15">
         <v>0</v>
       </c>
       <c r="J15">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K15">
         <v>0</v>
@@ -4153,19 +4153,19 @@
         <v>0</v>
       </c>
       <c r="M15">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N15">
         <v>0</v>
       </c>
       <c r="O15">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P15">
         <v>0</v>
       </c>
       <c r="Q15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R15">
         <v>0</v>
@@ -4213,13 +4213,13 @@
         <v>0</v>
       </c>
       <c r="AG15">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AH15">
         <v>0</v>
       </c>
       <c r="AI15">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AJ15">
         <v>0</v>
@@ -4234,10 +4234,10 @@
         <v>0</v>
       </c>
       <c r="AN15">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AO15">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:41">
@@ -4263,25 +4263,25 @@
         <v>0</v>
       </c>
       <c r="H16">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I16">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="J16">
         <v>0</v>
       </c>
       <c r="K16">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L16">
         <v>0</v>
       </c>
       <c r="M16">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N16">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O16">
         <v>0</v>
@@ -4370,7 +4370,7 @@
         <v>120</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -4495,7 +4495,7 @@
         <v>121</v>
       </c>
       <c r="B18">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -4510,13 +4510,13 @@
         <v>0</v>
       </c>
       <c r="G18">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H18">
         <v>0</v>
       </c>
       <c r="I18">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="J18">
         <v>0</v>
@@ -4737,7 +4737,7 @@
         <v>0</v>
       </c>
       <c r="AO19">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:41">
@@ -5862,7 +5862,7 @@
         <v>0</v>
       </c>
       <c r="AO28">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:41">
@@ -6016,7 +6016,7 @@
         <v>0</v>
       </c>
       <c r="I30">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="J30">
         <v>0</v>
@@ -6112,7 +6112,7 @@
         <v>0</v>
       </c>
       <c r="AO30">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:41">
@@ -7487,7 +7487,7 @@
         <v>0</v>
       </c>
       <c r="AO41">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:41">
@@ -8754,7 +8754,7 @@
         <v>0</v>
       </c>
       <c r="E52">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F52">
         <v>0</v>
@@ -8778,7 +8778,7 @@
         <v>0</v>
       </c>
       <c r="M52">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="N52">
         <v>0</v>
@@ -10011,7 +10011,7 @@
         <v>105</v>
       </c>
       <c r="B2">
-        <v>8680</v>
+        <v>560</v>
       </c>
       <c r="C2">
         <v>80</v>
@@ -10019,20 +10019,8 @@
       <c r="D2">
         <v>180</v>
       </c>
-      <c r="G2">
-        <v>480</v>
-      </c>
-      <c r="H2">
-        <v>580</v>
-      </c>
-      <c r="J2">
-        <v>780</v>
-      </c>
-      <c r="AB2">
-        <v>2600</v>
-      </c>
-      <c r="AP2">
-        <v>3980</v>
+      <c r="E2">
+        <v>300</v>
       </c>
     </row>
     <row r="3" spans="1:42">
@@ -10040,31 +10028,7 @@
         <v>106</v>
       </c>
       <c r="B3">
-        <v>6760</v>
-      </c>
-      <c r="C3">
-        <v>80</v>
-      </c>
-      <c r="D3">
-        <v>180</v>
-      </c>
-      <c r="E3">
-        <v>290</v>
-      </c>
-      <c r="F3">
-        <v>390</v>
-      </c>
-      <c r="G3">
-        <v>480</v>
-      </c>
-      <c r="H3">
-        <v>580</v>
-      </c>
-      <c r="J3">
-        <v>780</v>
-      </c>
-      <c r="AP3">
-        <v>3980</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:42">
@@ -10072,31 +10036,10 @@
         <v>107</v>
       </c>
       <c r="B4">
-        <v>7990</v>
-      </c>
-      <c r="C4">
-        <v>80</v>
-      </c>
-      <c r="D4">
-        <v>180</v>
-      </c>
-      <c r="E4">
-        <v>280</v>
+        <v>490</v>
       </c>
       <c r="G4">
         <v>490</v>
-      </c>
-      <c r="I4">
-        <v>690</v>
-      </c>
-      <c r="M4">
-        <v>1100</v>
-      </c>
-      <c r="N4">
-        <v>1190</v>
-      </c>
-      <c r="AP4">
-        <v>3980</v>
       </c>
     </row>
     <row r="5" spans="1:42">
@@ -10104,16 +10047,7 @@
         <v>108</v>
       </c>
       <c r="B5">
-        <v>900</v>
-      </c>
-      <c r="D5">
-        <v>200</v>
-      </c>
-      <c r="E5">
-        <v>300</v>
-      </c>
-      <c r="F5">
-        <v>400</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:42">
@@ -10121,25 +10055,7 @@
         <v>109</v>
       </c>
       <c r="B6">
-        <v>6550</v>
-      </c>
-      <c r="C6">
-        <v>100</v>
-      </c>
-      <c r="D6">
-        <v>200</v>
-      </c>
-      <c r="E6">
-        <v>300</v>
-      </c>
-      <c r="I6">
-        <v>680</v>
-      </c>
-      <c r="O6">
-        <v>1290</v>
-      </c>
-      <c r="AP6">
-        <v>3980</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:42">
@@ -10147,22 +10063,7 @@
         <v>110</v>
       </c>
       <c r="B7">
-        <v>7120</v>
-      </c>
-      <c r="G7">
-        <v>480</v>
-      </c>
-      <c r="I7">
-        <v>680</v>
-      </c>
-      <c r="J7">
-        <v>790</v>
-      </c>
-      <c r="N7">
-        <v>1190</v>
-      </c>
-      <c r="AP7">
-        <v>3980</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:42">
@@ -10170,22 +10071,7 @@
         <v>111</v>
       </c>
       <c r="B8">
-        <v>5050</v>
-      </c>
-      <c r="G8">
-        <v>490</v>
-      </c>
-      <c r="L8">
-        <v>1000</v>
-      </c>
-      <c r="M8">
-        <v>1080</v>
-      </c>
-      <c r="N8">
-        <v>1190</v>
-      </c>
-      <c r="O8">
-        <v>1290</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:42">
@@ -10193,25 +10079,7 @@
         <v>112</v>
       </c>
       <c r="B9">
-        <v>11010</v>
-      </c>
-      <c r="K9">
-        <v>880</v>
-      </c>
-      <c r="M9">
-        <v>1090</v>
-      </c>
-      <c r="P9">
-        <v>1380</v>
-      </c>
-      <c r="T9">
-        <v>1780</v>
-      </c>
-      <c r="U9">
-        <v>1900</v>
-      </c>
-      <c r="AP9">
-        <v>3980</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:42">
@@ -10219,22 +10087,7 @@
         <v>113</v>
       </c>
       <c r="B10">
-        <v>3640</v>
-      </c>
-      <c r="C10">
-        <v>100</v>
-      </c>
-      <c r="I10">
-        <v>690</v>
-      </c>
-      <c r="J10">
-        <v>780</v>
-      </c>
-      <c r="L10">
-        <v>980</v>
-      </c>
-      <c r="M10">
-        <v>1090</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:42">
@@ -10242,19 +10095,7 @@
         <v>114</v>
       </c>
       <c r="B11">
-        <v>10360</v>
-      </c>
-      <c r="Y11">
-        <v>2290</v>
-      </c>
-      <c r="AA11">
-        <v>2490</v>
-      </c>
-      <c r="AC11">
-        <v>2690</v>
-      </c>
-      <c r="AE11">
-        <v>2890</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:42">
@@ -10262,25 +10103,7 @@
         <v>115</v>
       </c>
       <c r="B12">
-        <v>16150</v>
-      </c>
-      <c r="H12">
-        <v>580</v>
-      </c>
-      <c r="J12">
-        <v>780</v>
-      </c>
-      <c r="AJ12">
-        <v>3400</v>
-      </c>
-      <c r="AL12">
-        <v>3600</v>
-      </c>
-      <c r="AN12">
-        <v>3800</v>
-      </c>
-      <c r="AP12">
-        <v>3990</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:42">
@@ -10288,22 +10111,7 @@
         <v>116</v>
       </c>
       <c r="B13">
-        <v>15760</v>
-      </c>
-      <c r="R13">
-        <v>1580</v>
-      </c>
-      <c r="AJ13">
-        <v>3400</v>
-      </c>
-      <c r="AK13">
-        <v>3490</v>
-      </c>
-      <c r="AL13">
-        <v>3590</v>
-      </c>
-      <c r="AM13">
-        <v>3700</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:42">
@@ -10311,31 +10119,7 @@
         <v>117</v>
       </c>
       <c r="B14">
-        <v>24540</v>
-      </c>
-      <c r="T14">
-        <v>1790</v>
-      </c>
-      <c r="AC14">
-        <v>2690</v>
-      </c>
-      <c r="AE14">
-        <v>2890</v>
-      </c>
-      <c r="AF14">
-        <v>3000</v>
-      </c>
-      <c r="AG14">
-        <v>3090</v>
-      </c>
-      <c r="AI14">
-        <v>3290</v>
-      </c>
-      <c r="AN14">
-        <v>3790</v>
-      </c>
-      <c r="AP14">
-        <v>4000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:42">
@@ -10343,40 +10127,7 @@
         <v>118</v>
       </c>
       <c r="B15">
-        <v>20580</v>
-      </c>
-      <c r="C15">
-        <v>80</v>
-      </c>
-      <c r="E15">
-        <v>280</v>
-      </c>
-      <c r="I15">
-        <v>690</v>
-      </c>
-      <c r="K15">
-        <v>890</v>
-      </c>
-      <c r="N15">
-        <v>1190</v>
-      </c>
-      <c r="P15">
-        <v>1390</v>
-      </c>
-      <c r="R15">
-        <v>1600</v>
-      </c>
-      <c r="AH15">
-        <v>3190</v>
-      </c>
-      <c r="AJ15">
-        <v>3390</v>
-      </c>
-      <c r="AO15">
-        <v>3890</v>
-      </c>
-      <c r="AP15">
-        <v>3990</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:42">
@@ -10384,64 +10135,34 @@
         <v>119</v>
       </c>
       <c r="B16">
-        <v>4930</v>
-      </c>
-      <c r="I16">
-        <v>690</v>
-      </c>
-      <c r="J16">
-        <v>780</v>
-      </c>
-      <c r="L16">
-        <v>980</v>
-      </c>
-      <c r="N16">
-        <v>1190</v>
-      </c>
-      <c r="O16">
-        <v>1290</v>
-      </c>
-    </row>
-    <row r="17" spans="1:42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
       <c r="A17" t="s">
         <v>120</v>
       </c>
       <c r="B17">
-        <v>100</v>
-      </c>
-      <c r="C17">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="18" spans="1:42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
       <c r="A18" t="s">
         <v>121</v>
       </c>
       <c r="B18">
-        <v>1440</v>
-      </c>
-      <c r="C18">
-        <v>80</v>
-      </c>
-      <c r="H18">
-        <v>580</v>
-      </c>
-      <c r="J18">
-        <v>780</v>
-      </c>
-    </row>
-    <row r="19" spans="1:42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
       <c r="A19" t="s">
         <v>122</v>
       </c>
       <c r="B19">
-        <v>3980</v>
-      </c>
-      <c r="AP19">
-        <v>3980</v>
-      </c>
-    </row>
-    <row r="20" spans="1:42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
       <c r="A20" t="s">
         <v>123</v>
       </c>
@@ -10449,7 +10170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:42">
+    <row r="21" spans="1:2">
       <c r="A21" t="s">
         <v>124</v>
       </c>
@@ -10457,7 +10178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:42">
+    <row r="22" spans="1:2">
       <c r="A22" t="s">
         <v>125</v>
       </c>
@@ -10465,7 +10186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:42">
+    <row r="23" spans="1:2">
       <c r="A23" t="s">
         <v>126</v>
       </c>
@@ -10473,7 +10194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:42">
+    <row r="24" spans="1:2">
       <c r="A24" t="s">
         <v>127</v>
       </c>
@@ -10481,7 +10202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:42">
+    <row r="25" spans="1:2">
       <c r="A25" t="s">
         <v>128</v>
       </c>
@@ -10489,7 +10210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:42">
+    <row r="26" spans="1:2">
       <c r="A26" t="s">
         <v>129</v>
       </c>
@@ -10497,7 +10218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:42">
+    <row r="27" spans="1:2">
       <c r="A27" t="s">
         <v>130</v>
       </c>
@@ -10505,18 +10226,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:42">
+    <row r="28" spans="1:2">
       <c r="A28" t="s">
         <v>131</v>
       </c>
       <c r="B28">
-        <v>3980</v>
-      </c>
-      <c r="AP28">
-        <v>3980</v>
-      </c>
-    </row>
-    <row r="29" spans="1:42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
       <c r="A29" t="s">
         <v>132</v>
       </c>
@@ -10524,21 +10242,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:42">
+    <row r="30" spans="1:2">
       <c r="A30" t="s">
         <v>133</v>
       </c>
       <c r="B30">
-        <v>4760</v>
-      </c>
-      <c r="J30">
-        <v>780</v>
-      </c>
-      <c r="AP30">
-        <v>3980</v>
-      </c>
-    </row>
-    <row r="31" spans="1:42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
       <c r="A31" t="s">
         <v>134</v>
       </c>
@@ -10546,7 +10258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:42">
+    <row r="32" spans="1:2">
       <c r="A32" t="s">
         <v>135</v>
       </c>
@@ -10554,7 +10266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:42">
+    <row r="33" spans="1:2">
       <c r="A33" t="s">
         <v>136</v>
       </c>
@@ -10562,7 +10274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:42">
+    <row r="34" spans="1:2">
       <c r="A34" t="s">
         <v>137</v>
       </c>
@@ -10570,7 +10282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:42">
+    <row r="35" spans="1:2">
       <c r="A35" t="s">
         <v>138</v>
       </c>
@@ -10578,7 +10290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:42">
+    <row r="36" spans="1:2">
       <c r="A36" t="s">
         <v>139</v>
       </c>
@@ -10586,7 +10298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:42">
+    <row r="37" spans="1:2">
       <c r="A37" t="s">
         <v>140</v>
       </c>
@@ -10594,7 +10306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:42">
+    <row r="38" spans="1:2">
       <c r="A38" t="s">
         <v>141</v>
       </c>
@@ -10602,7 +10314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:42">
+    <row r="39" spans="1:2">
       <c r="A39" t="s">
         <v>142</v>
       </c>
@@ -10610,7 +10322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:42">
+    <row r="40" spans="1:2">
       <c r="A40" t="s">
         <v>143</v>
       </c>
@@ -10618,18 +10330,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:42">
+    <row r="41" spans="1:2">
       <c r="A41" t="s">
         <v>144</v>
       </c>
       <c r="B41">
-        <v>3980</v>
-      </c>
-      <c r="AP41">
-        <v>3980</v>
-      </c>
-    </row>
-    <row r="42" spans="1:42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
       <c r="A42" t="s">
         <v>145</v>
       </c>
@@ -10637,7 +10346,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:42">
+    <row r="43" spans="1:2">
       <c r="A43" t="s">
         <v>146</v>
       </c>
@@ -10645,7 +10354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:42">
+    <row r="44" spans="1:2">
       <c r="A44" t="s">
         <v>147</v>
       </c>
@@ -10653,7 +10362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:42">
+    <row r="45" spans="1:2">
       <c r="A45" t="s">
         <v>148</v>
       </c>
@@ -10661,7 +10370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:42">
+    <row r="46" spans="1:2">
       <c r="A46" t="s">
         <v>149</v>
       </c>
@@ -10669,7 +10378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:42">
+    <row r="47" spans="1:2">
       <c r="A47" t="s">
         <v>150</v>
       </c>
@@ -10677,7 +10386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:42">
+    <row r="48" spans="1:2">
       <c r="A48" t="s">
         <v>151</v>
       </c>
@@ -10685,7 +10394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:14">
+    <row r="49" spans="1:2">
       <c r="A49" t="s">
         <v>152</v>
       </c>
@@ -10693,7 +10402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:14">
+    <row r="50" spans="1:2">
       <c r="A50" t="s">
         <v>153</v>
       </c>
@@ -10701,7 +10410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:14">
+    <row r="51" spans="1:2">
       <c r="A51" t="s">
         <v>154</v>
       </c>
@@ -10709,21 +10418,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:14">
+    <row r="52" spans="1:2">
       <c r="A52" t="s">
         <v>155</v>
       </c>
       <c r="B52">
-        <v>1560</v>
-      </c>
-      <c r="F52">
-        <v>380</v>
-      </c>
-      <c r="N52">
-        <v>1180</v>
-      </c>
-    </row>
-    <row r="53" spans="1:14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
       <c r="A53" t="s">
         <v>156</v>
       </c>
@@ -10731,7 +10434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:14">
+    <row r="54" spans="1:2">
       <c r="A54" t="s">
         <v>157</v>
       </c>
@@ -10739,7 +10442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:14">
+    <row r="55" spans="1:2">
       <c r="A55" t="s">
         <v>158</v>
       </c>
@@ -10747,7 +10450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:14">
+    <row r="56" spans="1:2">
       <c r="A56" t="s">
         <v>159</v>
       </c>
@@ -10755,7 +10458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:14">
+    <row r="57" spans="1:2">
       <c r="A57" t="s">
         <v>160</v>
       </c>
@@ -10763,7 +10466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:14">
+    <row r="58" spans="1:2">
       <c r="A58" t="s">
         <v>161</v>
       </c>
@@ -10771,7 +10474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:14">
+    <row r="59" spans="1:2">
       <c r="A59" t="s">
         <v>162</v>
       </c>
@@ -10779,7 +10482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:14">
+    <row r="60" spans="1:2">
       <c r="A60" t="s">
         <v>163</v>
       </c>

</xml_diff>